<commit_message>
Updated font sizes, updated layout
</commit_message>
<xml_diff>
--- a/data/Network Graph Data.xlsx
+++ b/data/Network Graph Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Node Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -431,7 +431,7 @@
     <t xml:space="preserve">Natsume Ooe</t>
   </si>
   <si>
-    <t xml:space="preserve">a student in Hisao's homeroom class who has rheumatoid arthritis and heterochromia that she wears glasses to compensate for the low vision in her right eye.</t>
+    <t xml:space="preserve">A student in Hisao's homeroom class who has rheumatoid arthritis and heterochromia that she wears glasses to compensate for the low vision in her right eye.</t>
   </si>
   <si>
     <t xml:space="preserve">#825A63</t>
@@ -1006,7 +1006,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1037,10 +1037,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1074,11 +1070,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ948"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G63" activeCellId="0" sqref="G63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.81"/>
@@ -1797,7 +1793,7 @@
       </c>
       <c r="G34" s="0" t="str">
         <f aca="false">"{""id"": """&amp;A34&amp;""", ""name"": """&amp;B34&amp;""", ""description"": """&amp;C34&amp;""", ""imageFilename"": """&amp;A34&amp;".png"", ""color"": """&amp;D34&amp;""", ""group"": """&amp;E34&amp;"""},"</f>
-        <v>{"id": "NATSUME_OOE", "name": "Natsume Ooe", "description": "a student in Hisao's homeroom class who has rheumatoid arthritis and heterochromia that she wears glasses to compensate for the low vision in her right eye.", "imageFilename": "NATSUME_OOE.png", "color": "#825A63", "group": "CHARACTER"},</v>
+        <v>{"id": "NATSUME_OOE", "name": "Natsume Ooe", "description": "A student in Hisao's homeroom class who has rheumatoid arthritis and heterochromia that she wears glasses to compensate for the low vision in her right eye.", "imageFilename": "NATSUME_OOE.png", "color": "#825A63", "group": "CHARACTER"},</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2448,11 +2444,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1201"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1179" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1119" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1202" activeCellId="0" sqref="D1202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.99"/>
@@ -3292,10 +3288,10 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="6" t="s">
         <v>210</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -3400,10 +3396,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="8" t="s">
         <v>213</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -3472,10 +3468,10 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="8" t="s">
         <v>217</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -3490,10 +3486,10 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="8" t="s">
         <v>217</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -3508,10 +3504,10 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="8" t="s">
         <v>217</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -3526,10 +3522,10 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="8" t="s">
         <v>219</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -3640,7 +3636,7 @@
       <c r="B66" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="C66" s="10"/>
+      <c r="C66" s="9"/>
       <c r="E66" s="2" t="s">
         <v>236</v>
       </c>
@@ -3656,7 +3652,7 @@
       <c r="B67" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="C67" s="10"/>
+      <c r="C67" s="9"/>
       <c r="E67" s="2" t="s">
         <v>236</v>
       </c>
@@ -3924,7 +3920,7 @@
       <c r="B82" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="C82" s="10" t="s">
         <v>263</v>
       </c>
       <c r="E82" s="2" t="s">
@@ -3942,7 +3938,7 @@
       <c r="B83" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="C83" s="10" t="s">
         <v>264</v>
       </c>
       <c r="E83" s="2" t="s">
@@ -3960,7 +3956,7 @@
       <c r="B84" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C84" s="11" t="s">
+      <c r="C84" s="10" t="s">
         <v>265</v>
       </c>
       <c r="E84" s="2" t="s">
@@ -3978,7 +3974,7 @@
       <c r="B85" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C85" s="11" t="s">
+      <c r="C85" s="10" t="s">
         <v>266</v>
       </c>
       <c r="E85" s="2" t="s">
@@ -3996,7 +3992,7 @@
       <c r="B86" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="C86" s="10" t="s">
         <v>267</v>
       </c>
       <c r="E86" s="2" t="s">
@@ -7014,7 +7010,7 @@
       <c r="B280" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C280" s="10" t="s">
+      <c r="C280" s="9" t="s">
         <v>285</v>
       </c>
       <c r="E280" s="2" t="s">
@@ -7152,7 +7148,7 @@
       <c r="B289" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C289" s="10"/>
+      <c r="C289" s="9"/>
       <c r="E289" s="2" t="s">
         <v>257</v>
       </c>
@@ -7978,7 +7974,7 @@
       <c r="B342" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C342" s="11"/>
+      <c r="C342" s="10"/>
       <c r="E342" s="2" t="s">
         <v>257</v>
       </c>
@@ -8054,7 +8050,7 @@
       <c r="B347" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C347" s="10" t="s">
+      <c r="C347" s="9" t="s">
         <v>262</v>
       </c>
       <c r="E347" s="2" t="s">
@@ -15299,7 +15295,7 @@
       <c r="A827" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B827" s="10" t="s">
+      <c r="B827" s="9" t="s">
         <v>110</v>
       </c>
       <c r="E827" s="2" t="s">
@@ -15314,7 +15310,7 @@
       <c r="A828" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B828" s="10" t="s">
+      <c r="B828" s="9" t="s">
         <v>114</v>
       </c>
       <c r="E828" s="2" t="s">
@@ -15329,7 +15325,7 @@
       <c r="A829" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B829" s="10" t="s">
+      <c r="B829" s="9" t="s">
         <v>118</v>
       </c>
       <c r="E829" s="2" t="s">
@@ -15344,7 +15340,7 @@
       <c r="A830" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B830" s="10" t="s">
+      <c r="B830" s="9" t="s">
         <v>122</v>
       </c>
       <c r="E830" s="2" t="s">
@@ -15359,7 +15355,7 @@
       <c r="A831" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B831" s="10" t="s">
+      <c r="B831" s="9" t="s">
         <v>126</v>
       </c>
       <c r="E831" s="2" t="s">
@@ -15374,7 +15370,7 @@
       <c r="A832" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B832" s="10" t="s">
+      <c r="B832" s="9" t="s">
         <v>130</v>
       </c>
       <c r="E832" s="2" t="s">
@@ -15389,7 +15385,7 @@
       <c r="A833" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B833" s="10" t="s">
+      <c r="B833" s="9" t="s">
         <v>134</v>
       </c>
       <c r="E833" s="2" t="s">

</xml_diff>